<commit_message>
Added new exeption catching. Changed json files
</commit_message>
<xml_diff>
--- a/src/excel_files/png/jp/import/PNGLO001R_IMPORT_SO_TESTING_png_i_b_nd_pl_fcl.xlsx
+++ b/src/excel_files/png/jp/import/PNGLO001R_IMPORT_SO_TESTING_png_i_b_nd_pl_fcl.xlsx
@@ -834,17 +834,17 @@
     <row r="3">
       <c r="A3" s="13" t="inlineStr">
         <is>
-          <t>JSSO1000219</t>
+          <t>JSSO1000243</t>
         </is>
       </c>
       <c r="B3" s="13" t="inlineStr">
         <is>
-          <t>JSSO1000219</t>
+          <t>JSSO1000243</t>
         </is>
       </c>
       <c r="C3" s="13" t="inlineStr">
         <is>
-          <t>JSSO1000219</t>
+          <t>JSSO1000243</t>
         </is>
       </c>
       <c r="D3" s="18" t="inlineStr">
@@ -980,7 +980,7 @@
       </c>
       <c r="AJ3" s="17" t="inlineStr">
         <is>
-          <t>JSCN1000219</t>
+          <t>JSCN1000243</t>
         </is>
       </c>
       <c r="AK3" s="20" t="inlineStr">
@@ -990,7 +990,7 @@
       </c>
       <c r="AL3" s="20" t="inlineStr">
         <is>
-          <t>SLJSSO1000219</t>
+          <t>SLJSSO1000243</t>
         </is>
       </c>
       <c r="AM3" s="20" t="inlineStr">
@@ -1000,7 +1000,7 @@
       </c>
       <c r="AN3" s="20" t="inlineStr">
         <is>
-          <t>JSCN1000219</t>
+          <t>JSCN1000243</t>
         </is>
       </c>
       <c r="AP3" s="20" t="inlineStr">

</xml_diff>